<commit_message>
Contribution sheet updated for week 4
</commit_message>
<xml_diff>
--- a/docs/Contribution Spreadsheet SET09623 (Group 2).xlsx
+++ b/docs/Contribution Spreadsheet SET09623 (Group 2).xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bsc (Hons)\DevOps\Coursework-group2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bsc (Hons)\DevOps\Coursework-group2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED62921-2A4C-4FD9-BBA9-40BE6044769E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD2DA1B-C1B2-4875-A3A3-7206DA502837}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8880" xr2:uid="{7C81EAE5-9AC4-4E43-98CD-A19758BE81E9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Group 2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -428,7 +428,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,6 +481,9 @@
       <c r="E2">
         <v>25</v>
       </c>
+      <c r="F2">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -498,6 +501,9 @@
       <c r="E3">
         <v>25</v>
       </c>
+      <c r="F3">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -515,6 +521,9 @@
       <c r="E4">
         <v>25</v>
       </c>
+      <c r="F4">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -532,6 +541,9 @@
       <c r="E5">
         <v>25</v>
       </c>
+      <c r="F5">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -551,7 +563,7 @@
       </c>
       <c r="F7">
         <f>SUM(F2,F3,F4,F5)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G7">
         <f>SUM(G2,G3,G4,G5)</f>

</xml_diff>

<commit_message>
readme and contribution updated
</commit_message>
<xml_diff>
--- a/docs/Contribution Spreadsheet SET09623 (Group 2).xlsx
+++ b/docs/Contribution Spreadsheet SET09623 (Group 2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bsc (Hons)\DevOps\Coursework-group2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD2DA1B-C1B2-4875-A3A3-7206DA502837}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11A18B7-8F00-4C99-BAEC-7D489FB4D606}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8880" xr2:uid="{7C81EAE5-9AC4-4E43-98CD-A19758BE81E9}"/>
   </bookViews>
@@ -428,7 +428,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,6 +484,9 @@
       <c r="F2">
         <v>25</v>
       </c>
+      <c r="G2">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -504,6 +507,9 @@
       <c r="F3">
         <v>25</v>
       </c>
+      <c r="G3">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -524,6 +530,9 @@
       <c r="F4">
         <v>25</v>
       </c>
+      <c r="G4">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -544,6 +553,9 @@
       <c r="F5">
         <v>25</v>
       </c>
+      <c r="G5">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -567,7 +579,7 @@
       </c>
       <c r="G7">
         <f>SUM(G2,G3,G4,G5)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>